<commit_message>
code refactoring of EXF
</commit_message>
<xml_diff>
--- a/src/main/java/lomt/pearson/fileupload/externalframework/ex_reingestion/External_Framework_Template.xlsx
+++ b/src/main/java/lomt/pearson/fileupload/externalframework/ex_reingestion/External_Framework_Template.xlsx
@@ -12,12 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="172">
-  <si>
-    <t>External Frameworks_all_fields_with_metadata_A007_Updated-369</t>
-  </si>
-  <si>
-    <t>urn:pearson:goalframework:41393e29-6a87-417f-a36b-0ec9f0ea9249</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="176">
+  <si>
+    <t>Australia Citizenship PK-12 2092</t>
+  </si>
+  <si>
+    <t>urn:pearson:goalframework:b0d11c76-9e0a-47b9-bf0c-cc40c63f6f3f</t>
   </si>
   <si>
     <t>Unique id</t>
@@ -47,7 +47,7 @@
     <t>Tags</t>
   </si>
   <si>
-    <t>urn:pearson:educationalgoal:3084f96a-4f00-4d14-92fd-b99a3350f050</t>
+    <t>urn:pearson:educationalgoal:6677bb6d-7fa4-4308-9112-05c82bda4c6d</t>
   </si>
   <si>
     <t>K</t>
@@ -56,16 +56,16 @@
     <t>11</t>
   </si>
   <si>
-    <t>Grade Title !@$%^&amp;*()_+{}|:';&lt;&gt;?Test123456Updated-42</t>
-  </si>
-  <si>
-    <t>CCE A !@$%^&amp;*()_+{}|:';&lt;&gt;?Test123456Updated-44</t>
-  </si>
-  <si>
-    <t>Ability to apply the process of science ExternalFramework!@$%^&amp;*()_+{}|:';&lt;&gt;?Test123456Updated-19</t>
-  </si>
-  <si>
-    <t>urn:pearson:educationalgoal:ee658173-c9e6-484c-9c69-fd9b29591b92</t>
+    <t>CCE A !@$%^&amp;*()_+{}|:';&lt;&gt;?Test123456Updated-60</t>
+  </si>
+  <si>
+    <t>Ability to apply the process of science ExternalFramework!@$%^&amp;*()_+{}|:';&lt;&gt;?Test123456Updated-29</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>urn:pearson:educationalgoal:98b3cc4a-680a-4233-bbef-af78c9bf864b</t>
   </si>
   <si>
     <t>PK</t>
@@ -74,7 +74,7 @@
     <t>10</t>
   </si>
   <si>
-    <t>urn:pearson:educationalgoal:633cd156-61a2-4ec5-965b-6f52d505f1b8</t>
+    <t>urn:pearson:educationalgoal:8c32b531-b2d3-4cee-aaa7-804cabcfd008</t>
   </si>
   <si>
     <t>1</t>
@@ -83,37 +83,34 @@
     <t>12</t>
   </si>
   <si>
-    <t>AAAS</t>
-  </si>
-  <si>
     <t>CCE A1.1</t>
   </si>
   <si>
-    <t>Instantiation of Ability in Disciplinary Practice ExternalFramework!@$%^&amp;*()_+{}|:';&lt;&gt;?Test123456Updated-73</t>
-  </si>
-  <si>
-    <t>urn:pearson:educationalgoal:7f87b8ab-b44c-447f-9592-b6defdbd3ad6</t>
+    <t>Instantiation of Ability in Disciplinary Practice ExternalFramework!@$%^&amp;*()_+{}|:';&lt;&gt;?Test123456Updated-69</t>
+  </si>
+  <si>
+    <t>urn:pearson:educationalgoal:280bb343-f8dd-43f6-998a-88daeda60485</t>
   </si>
   <si>
     <t>CCE A1.1.1</t>
   </si>
   <si>
-    <t>Biology is an evidence-based discipline ExternalFramework!@$%^&amp;*()_+{}|:';&lt;&gt;?Test123456Updated-72</t>
-  </si>
-  <si>
-    <t>urn:pearson:educationalgoal:387a9edc-5b84-48c3-ac51-e4a31c0ef247</t>
+    <t>Biology is an evidence-based discipline ExternalFramework!@$%^&amp;*()_+{}|:';&lt;&gt;?Test123456Updated-80</t>
+  </si>
+  <si>
+    <t>urn:pearson:educationalgoal:164133f4-6af0-47ab-b230-8b5bb8a4cdf5</t>
   </si>
   <si>
     <t>CCE A1.2</t>
   </si>
   <si>
-    <t>urn:pearson:educationalgoal:1e5a8dcc-3a85-494d-a16c-e90a3b9dea31</t>
+    <t>urn:pearson:educationalgoal:f98dd527-c985-41be-ab47-3c380ca2587e</t>
   </si>
   <si>
     <t>CCE A1.2.1</t>
   </si>
   <si>
-    <t>urn:pearson:educationalgoal:8bb14ff8-2000-4b44-a65d-d6f5c4c4d03b</t>
+    <t>urn:pearson:educationalgoal:6395e36b-8c08-4a34-bd40-f00e96367d05</t>
   </si>
   <si>
     <t>CCE A1.3</t>
@@ -122,7 +119,7 @@
     <t>Examples of Core Competencies Applied to Biology Practice</t>
   </si>
   <si>
-    <t>urn:pearson:educationalgoal:1c6819a0-6393-40a6-81ec-34067a84e038</t>
+    <t>urn:pearson:educationalgoal:7e4c3238-8fdf-48f6-8059-664f46c7052e</t>
   </si>
   <si>
     <t>CCE A1.3.1</t>
@@ -131,10 +128,7 @@
     <t>Observational strategies</t>
   </si>
   <si>
-    <t>urn:pearson:educationalgoal:8e76f99e-bee5-43ef-a4a7-735757f64e67</t>
-  </si>
-  <si>
-    <t/>
+    <t>urn:pearson:educationalgoal:02ef324d-f343-428a-af45-6eee16049457</t>
   </si>
   <si>
     <t>CCE A1.3.2</t>
@@ -143,7 +137,7 @@
     <t>Hypothesis testing</t>
   </si>
   <si>
-    <t>urn:pearson:educationalgoal:e37233fd-a15f-4737-8d99-edeebfcfe817</t>
+    <t>urn:pearson:educationalgoal:7117c924-c677-4ab5-9f39-a25706ac7946</t>
   </si>
   <si>
     <t>CCE A1.3.3</t>
@@ -152,7 +146,7 @@
     <t>Experimental design</t>
   </si>
   <si>
-    <t>urn:pearson:educationalgoal:dd844db9-e134-4b92-8cc9-a83fc690a181</t>
+    <t>urn:pearson:educationalgoal:cb9ede6c-a6e8-42f3-864a-426bb94252be</t>
   </si>
   <si>
     <t>CCE A1.3.4</t>
@@ -161,7 +155,7 @@
     <t>Evaluation of experimental evidence</t>
   </si>
   <si>
-    <t>urn:pearson:educationalgoal:e9adf21f-ad81-4cc2-8be7-775d161d4134</t>
+    <t>urn:pearson:educationalgoal:5aa3f509-7895-4a64-b0fe-07078c6f54d8</t>
   </si>
   <si>
     <t>CCE A1.3.5</t>
@@ -170,7 +164,7 @@
     <t>Developing problem-solving strategies</t>
   </si>
   <si>
-    <t>urn:pearson:educationalgoal:23dce832-96aa-4870-b562-da452ee82c57</t>
+    <t>urn:pearson:educationalgoal:f3c3ae68-fbe0-4268-a1eb-80f04789da98</t>
   </si>
   <si>
     <t>CCE A2</t>
@@ -179,7 +173,7 @@
     <t>Ability to use quantitative reasoning</t>
   </si>
   <si>
-    <t>urn:pearson:educationalgoal:11d221cf-0961-44ad-86c7-7dfd30c9d2dd</t>
+    <t>urn:pearson:educationalgoal:c21572ec-6b93-4728-892f-81bfaeac924b</t>
   </si>
   <si>
     <t>CCE A2.1</t>
@@ -188,7 +182,7 @@
     <t>Instantiation of Ability in Disciplinary Practice</t>
   </si>
   <si>
-    <t>urn:pearson:educationalgoal:33214be1-a0bb-4d3a-991d-b41ca735dffc</t>
+    <t>urn:pearson:educationalgoal:70500c40-3c66-43c8-a8ee-317ff073fbe6</t>
   </si>
   <si>
     <t>CCE A2.1.1</t>
@@ -197,7 +191,7 @@
     <t>Biology relies on applications of quantitative analysis and mathematical reasoning</t>
   </si>
   <si>
-    <t>urn:pearson:educationalgoal:a35d9815-e177-45ee-abc3-140dec948228</t>
+    <t>urn:pearson:educationalgoal:de2b046e-3033-4872-8e6f-ab46c49bb5df</t>
   </si>
   <si>
     <t>CCE A2.2</t>
@@ -206,7 +200,7 @@
     <t>Demonstration of Competency in Practice</t>
   </si>
   <si>
-    <t>urn:pearson:educationalgoal:660bf374-7e4f-467e-a4c7-f7b63efce46c</t>
+    <t>urn:pearson:educationalgoal:062d7010-bbd6-4de8-b2ac-8e64a51bd1ed</t>
   </si>
   <si>
     <t>CCE A2.2.1</t>
@@ -215,13 +209,13 @@
     <t>Apply quantitative analysis to interpret biological data</t>
   </si>
   <si>
-    <t>urn:pearson:educationalgoal:75ea2de6-cd7f-4204-b6f6-7b7a186112b4</t>
+    <t>urn:pearson:educationalgoal:546cc959-931f-432f-9034-6856cb80dabc</t>
   </si>
   <si>
     <t>CCE A2.3</t>
   </si>
   <si>
-    <t>urn:pearson:educationalgoal:5f2084b8-002a-4a09-836e-b76845e4d546</t>
+    <t>urn:pearson:educationalgoal:82a36edf-e982-4d38-beda-b1e1be10c464</t>
   </si>
   <si>
     <t>CCE A2.3.1</t>
@@ -230,7 +224,7 @@
     <t>Developing and interpreting graphs</t>
   </si>
   <si>
-    <t>urn:pearson:educationalgoal:7236bdef-a12d-455e-a25d-7fd8df9b7258</t>
+    <t>urn:pearson:educationalgoal:38f5f77e-d39f-4092-a083-369b0c3c22fb</t>
   </si>
   <si>
     <t>CCE A2.3.2</t>
@@ -239,7 +233,7 @@
     <t>Applying statistical methods to diverse data</t>
   </si>
   <si>
-    <t>urn:pearson:educationalgoal:fd1a02ee-66f5-480f-9d15-1610fba38be5</t>
+    <t>urn:pearson:educationalgoal:a54b9883-0625-4175-b982-b52927cc9f2b</t>
   </si>
   <si>
     <t>CCE A2.3.3</t>
@@ -248,7 +242,7 @@
     <t>Mathematical modeling</t>
   </si>
   <si>
-    <t>urn:pearson:educationalgoal:108c2c0b-3ef3-42b9-ad51-156bc16eb234</t>
+    <t>urn:pearson:educationalgoal:e43cfe82-f6e1-4188-8fb0-eba23303b719</t>
   </si>
   <si>
     <t>CCE A2.3.4</t>
@@ -257,7 +251,7 @@
     <t>Managing and analyzing large data sets</t>
   </si>
   <si>
-    <t>urn:pearson:educationalgoal:1bbef4f8-9e5b-43e7-a4cd-aa389dde9dee</t>
+    <t>urn:pearson:educationalgoal:62ac95c6-9603-46ea-bf24-3e45c7f50e9b</t>
   </si>
   <si>
     <t>CCE A3</t>
@@ -266,13 +260,13 @@
     <t>Ability to use modeling and simulation</t>
   </si>
   <si>
-    <t>urn:pearson:educationalgoal:2ea368a6-b425-4a2f-9381-1891cd4f6492</t>
+    <t>urn:pearson:educationalgoal:3ff0eef5-3fb5-4bd3-b4e0-8ba1f1b393ac</t>
   </si>
   <si>
     <t>CCE A3.1</t>
   </si>
   <si>
-    <t>urn:pearson:educationalgoal:67268654-2679-429e-afec-cc50f36e7955</t>
+    <t>urn:pearson:educationalgoal:92841445-b7eb-4459-b792-89cfa065e11d</t>
   </si>
   <si>
     <t>CCE A3.1.1</t>
@@ -281,13 +275,13 @@
     <t>Biology focuses on the study of complex systems</t>
   </si>
   <si>
-    <t>urn:pearson:educationalgoal:d9236bf0-c00e-4357-9478-20ef4312eb41</t>
+    <t>urn:pearson:educationalgoal:3af1fd5e-a889-44a7-affb-fa9b58de1a73</t>
   </si>
   <si>
     <t>CCE A3.2</t>
   </si>
   <si>
-    <t>urn:pearson:educationalgoal:9cd6fb59-109f-4ebb-afd9-e3112c43eb4f</t>
+    <t>urn:pearson:educationalgoal:6b619265-b5ff-4a31-9e61-e36bf4132b40</t>
   </si>
   <si>
     <t>CCE A3.2.1</t>
@@ -296,13 +290,13 @@
     <t>Use mathematical modeling and simulation tools to describe living systems</t>
   </si>
   <si>
-    <t>urn:pearson:educationalgoal:f0cd63d3-316f-42f4-9f55-976af07ac199</t>
+    <t>urn:pearson:educationalgoal:cc88dd74-1dd3-4e64-83c0-86be498ccedc</t>
   </si>
   <si>
     <t>CCE A3.3</t>
   </si>
   <si>
-    <t>urn:pearson:educationalgoal:23c602cb-b233-47fa-a7b4-c1b055068b54</t>
+    <t>urn:pearson:educationalgoal:9da4733c-ab09-4f18-9049-2f17aa15e489</t>
   </si>
   <si>
     <t>CCE A3.3.1</t>
@@ -311,7 +305,7 @@
     <t>Computational modeling of dynamic systems</t>
   </si>
   <si>
-    <t>urn:pearson:educationalgoal:b64a6a28-1626-404f-a68c-1da190df677d</t>
+    <t>urn:pearson:educationalgoal:46249a6f-b2f5-4886-a0de-c0926179810a</t>
   </si>
   <si>
     <t>CCE A3.3.2</t>
@@ -320,7 +314,7 @@
     <t>and so on</t>
   </si>
   <si>
-    <t>urn:pearson:educationalgoal:f267f575-7684-430a-89a3-ed104c42ce42</t>
+    <t>urn:pearson:educationalgoal:be74104d-1040-4646-85d7-b177c34581eb</t>
   </si>
   <si>
     <t>CCE B</t>
@@ -329,13 +323,13 @@
     <t>Core Sequence Example B</t>
   </si>
   <si>
-    <t>urn:pearson:educationalgoal:add51b1d-a5ba-4f7e-b42d-a96cf3d390aa</t>
+    <t>urn:pearson:educationalgoal:43153009-ee5e-47d9-bfa9-b9c9f050b617</t>
   </si>
   <si>
     <t>CCE B1</t>
   </si>
   <si>
-    <t>urn:pearson:educationalgoal:3d91d306-fc40-4091-929b-295a17459832</t>
+    <t>urn:pearson:educationalgoal:11a7d08d-849d-4ef3-9455-f2cecccbf5e2</t>
   </si>
   <si>
     <t>CCE B1.1</t>
@@ -344,7 +338,7 @@
     <t>Ability to apply the process of science</t>
   </si>
   <si>
-    <t>urn:pearson:educationalgoal:16f30ca5-f2de-4249-9fa2-9d7d1409065e</t>
+    <t>urn:pearson:educationalgoal:e769d223-67e5-4243-addb-3dfe53a8e929</t>
   </si>
   <si>
     <t>CCE B1.1.1</t>
@@ -353,31 +347,31 @@
     <t>Biology is an evidence-based discipline</t>
   </si>
   <si>
-    <t>urn:pearson:educationalgoal:e0f3351a-79f5-40e2-bfa5-4f35560dcead</t>
+    <t>urn:pearson:educationalgoal:18fe7c47-8e48-478a-bd36-1e5d1373a96b</t>
   </si>
   <si>
     <t>CCE B1.2</t>
   </si>
   <si>
-    <t>urn:pearson:educationalgoal:41bc93aa-84f6-4c32-9d1c-c066897fe110</t>
+    <t>urn:pearson:educationalgoal:76b552fc-106e-4697-8ef2-592bc7da0df4</t>
   </si>
   <si>
     <t>CCE B1.2.1</t>
   </si>
   <si>
-    <t>urn:pearson:educationalgoal:435d696c-66f0-4901-b78c-2c00b74dc51e</t>
+    <t>urn:pearson:educationalgoal:764fa47d-2313-42d5-851a-506e0416c9f7</t>
   </si>
   <si>
     <t>CCE B1.3</t>
   </si>
   <si>
-    <t>urn:pearson:educationalgoal:3963b96d-97e2-41fd-871b-d3e72229d01e</t>
+    <t>urn:pearson:educationalgoal:f49342ee-6721-45ad-b695-d3b27a3ffdd9</t>
   </si>
   <si>
     <t>CCE B1.3.1</t>
   </si>
   <si>
-    <t>urn:pearson:educationalgoal:faa52dd4-882e-40fa-bf34-cb0e00c6a342</t>
+    <t>urn:pearson:educationalgoal:edc3b7ec-b551-41ee-966b-d290cfac6cb5</t>
   </si>
   <si>
     <t>CCE B1.4</t>
@@ -386,19 +380,19 @@
     <t>Ability to tap into the interdisciplinary nature of science</t>
   </si>
   <si>
-    <t>urn:pearson:educationalgoal:a3f66139-bd1c-4164-a29d-a66568c773c4</t>
+    <t>urn:pearson:educationalgoal:7f57925f-96d8-4921-9c38-4cea2c30df5f</t>
   </si>
   <si>
     <t>CCE B2</t>
   </si>
   <si>
-    <t>urn:pearson:educationalgoal:1375a403-8908-45b8-b2d8-09ce9f937df5</t>
+    <t>urn:pearson:educationalgoal:c63b66f9-15e0-4790-8eea-572d60025782</t>
   </si>
   <si>
     <t>CCE B2.1</t>
   </si>
   <si>
-    <t>urn:pearson:educationalgoal:19d6782d-81cb-44ea-866c-7ff58ae751ff</t>
+    <t>urn:pearson:educationalgoal:3d59fcae-b760-4b43-8477-7adfc57d1cef</t>
   </si>
   <si>
     <t>CCE B2.1.1</t>
@@ -407,127 +401,145 @@
     <t>Design scientific process to understand living systems</t>
   </si>
   <si>
-    <t>urn:pearson:educationalgoal:30158a69-6ec1-4d93-97bc-2e2d3c36e5a1</t>
+    <t>urn:pearson:educationalgoal:3eb2e86d-325c-4289-9c09-e515cb33ab20</t>
   </si>
   <si>
     <t>CCE B2.2</t>
   </si>
   <si>
-    <t>urn:pearson:educationalgoal:266dc143-c79c-4459-974c-3544b9685bbd</t>
+    <t>urn:pearson:educationalgoal:f6196c45-64d0-47cf-9f7d-e5e8ec2776f1</t>
   </si>
   <si>
     <t>CCE B2.2.1</t>
   </si>
   <si>
-    <t>urn:pearson:educationalgoal:1fd41223-42ca-40d5-9497-ca21bd1264cb</t>
+    <t>urn:pearson:educationalgoal:1ca0b2c1-2873-4b42-b86f-ec7d0bbf6e74</t>
   </si>
   <si>
     <t>CCE B2.3</t>
   </si>
   <si>
-    <t>urn:pearson:educationalgoal:e4399c32-c8a6-4353-a02f-a4c84ce173cd</t>
+    <t>urn:pearson:educationalgoal:4c6127c1-621c-46e6-815b-f3abe0a442ac</t>
   </si>
   <si>
     <t>CCE B2.3.1</t>
   </si>
   <si>
-    <t>urn:pearson:educationalgoal:b951df8a-e3ef-4c0c-92ef-7c62467f3a1e</t>
+    <t>urn:pearson:educationalgoal:d8be8a2c-a968-426e-8c1b-f24856efb26b</t>
   </si>
   <si>
     <t>CCE B2.4</t>
   </si>
   <si>
-    <t>urn:pearson:educationalgoal:a8afee5f-9fbb-400b-8794-8d51c5ad960c</t>
+    <t>urn:pearson:educationalgoal:52739dff-06e9-4645-8566-24df6fa870b2</t>
   </si>
   <si>
     <t>CCE B3</t>
   </si>
   <si>
-    <t>urn:pearson:educationalgoal:a1da8b2e-2a71-4d09-983f-c9cd18f6ccda</t>
+    <t>urn:pearson:educationalgoal:10147f8d-5a54-4c24-9cd4-d685414404ef</t>
   </si>
   <si>
     <t>CCE B3.1</t>
   </si>
   <si>
-    <t>urn:pearson:educationalgoal:4db4aefd-efc0-43aa-921c-ee15a024ed73</t>
+    <t>urn:pearson:educationalgoal:195eb3ef-348c-47c4-9bc0-656af6b1f8c2</t>
   </si>
   <si>
     <t>CCE B3.1.1</t>
   </si>
   <si>
-    <t>urn:pearson:educationalgoal:1287a8d2-fb63-4754-8c18-ef84b492e3f7</t>
+    <t>urn:pearson:educationalgoal:b044113a-32d3-4091-9603-f1cde719b89a</t>
   </si>
   <si>
     <t>CCE B3.1.2</t>
   </si>
   <si>
-    <t>urn:pearson:educationalgoal:6bccce51-37cf-47e0-a329-d23ec7133eb0</t>
+    <t>urn:pearson:educationalgoal:33b61299-e833-4ebc-aab1-b4ad6924a0bd</t>
   </si>
   <si>
     <t>CCE B3.1.3</t>
   </si>
   <si>
-    <t>urn:pearson:educationalgoal:1a258c4a-50f2-4063-8442-65367d6f797f</t>
+    <t>urn:pearson:educationalgoal:2d4c02a9-27dc-4230-b118-df134741536f</t>
   </si>
   <si>
     <t>CCE B3.1.4</t>
   </si>
   <si>
-    <t>urn:pearson:educationalgoal:6523a15f-65ae-45c8-ac4c-2183661a260e</t>
+    <t>urn:pearson:educationalgoal:bea3e0b6-5a05-4c39-8eb9-e11985141dc4</t>
   </si>
   <si>
     <t>CCE B3.1.5</t>
   </si>
   <si>
-    <t>urn:pearson:educationalgoal:ff8515af-a333-4576-8b09-85947db3ad86</t>
+    <t>urn:pearson:educationalgoal:6be21cbe-d643-467a-b26d-9d08c4dc38c3</t>
   </si>
   <si>
     <t>CCE B3.2</t>
   </si>
   <si>
-    <t>urn:pearson:educationalgoal:45a874e9-d075-43bd-bb64-bbb33c7ce346</t>
+    <t>urn:pearson:educationalgoal:742d7e29-e61d-4020-a242-522c3ddf1ed7</t>
   </si>
   <si>
     <t>CCE B3.2.1</t>
   </si>
   <si>
-    <t>urn:pearson:educationalgoal:11bc1fa8-3d8d-4f30-8fb4-cb19bc131534</t>
+    <t>urn:pearson:educationalgoal:a2c7e6f4-fa18-4e06-a0ad-90baa6016d00</t>
   </si>
   <si>
     <t>CCE B3.2.2</t>
   </si>
   <si>
-    <t>urn:pearson:educationalgoal:047d622b-65d7-4abf-839a-1009eaf5ade4</t>
+    <t>urn:pearson:educationalgoal:e31d8e45-2e90-445d-bd01-38819944ea07</t>
   </si>
   <si>
     <t>CCE B3.2.3</t>
   </si>
   <si>
-    <t>urn:pearson:educationalgoal:c5b9ebc4-5ca2-4cf2-ab19-6c2e3b009ef3</t>
+    <t>urn:pearson:educationalgoal:de32fb02-b25f-40fc-a737-e37a38e65aab</t>
   </si>
   <si>
     <t>CCE B3.2.4</t>
   </si>
   <si>
-    <t>urn:pearson:educationalgoal:7e62ccbe-a231-4c2c-a7eb-5be9b44eeca6</t>
+    <t>urn:pearson:educationalgoal:adf92ddf-5ec8-4753-ba54-71d951e0bfb9</t>
   </si>
   <si>
     <t>CCE B3.3</t>
   </si>
   <si>
-    <t>urn:pearson:educationalgoal:d031501a-5600-4ddc-9094-be81d3419261</t>
+    <t>urn:pearson:educationalgoal:497cc645-aa37-40d8-a3d6-14e91f227ed6</t>
   </si>
   <si>
     <t>CCE B3.3.1</t>
   </si>
   <si>
-    <t>urn:pearson:educationalgoal:d47ff024-f93e-455e-b2e0-fd34bbb688f4</t>
+    <t>urn:pearson:educationalgoal:01f9605c-abaf-43de-95ca-df28620ce275</t>
   </si>
   <si>
     <t>CCE B3.3.3</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
+    <t>AAAS NEW ADDED GRADE Title</t>
+  </si>
+  <si>
+    <t>CCE A1.0 NEW ADDED Off Std. Code</t>
+  </si>
+  <si>
+    <t>Core Sequence Example B - NEW ADDED</t>
+  </si>
+  <si>
+    <t>AAAS NEW ADDED GRADE Title !@#$%^&amp;*()_+{}|',./?&gt;&lt;123</t>
+  </si>
+  <si>
+    <t>CCE A1.0 NEW ADDED Off Std. Code !@#$%^&amp;*()_+{}|',./?&gt;&lt;123</t>
+  </si>
+  <si>
+    <t>LEVEL 2 Biology relies on applications of quantitative analysis and mathematical reasoning!@#$%^&amp;*()_+{}|',./?&gt;&lt;123 - NEW ADDED</t>
+  </si>
+  <si>
+    <t>LOWEST LEVEL Biology relies on applications of quantitative analysis and mathematical reasoning!@#$%^&amp;*()_+{}|',./?&gt;&lt;123 - NEW ADDED</t>
   </si>
 </sst>
 </file>
@@ -646,9 +658,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="65.6953125" collapsed="false"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="64.17578125" collapsed="false"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="12.8046875" collapsed="false"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="55.4765625" collapsed="false"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.65234375" collapsed="false"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="50.875" collapsed="false"/>
     <col min="6" max="6" bestFit="true" customWidth="true" width="98.1328125" collapsed="false"/>
     <col min="7" max="7" bestFit="true" customWidth="true" width="104.921875" collapsed="false"/>
@@ -658,7 +670,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>171</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -703,146 +715,134 @@
       <c r="C3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3"/>
+      <c r="E3" t="s">
         <v>14</v>
       </c>
-      <c r="E3" t="s">
-        <v>171</v>
-      </c>
       <c r="F3" t="s">
-        <v>171</v>
-      </c>
-      <c r="I3"/>
+        <v>15</v>
+      </c>
+      <c r="I3" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" t="s">
-        <v>17</v>
-      </c>
       <c r="B4" t="s">
         <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>169</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>170</v>
       </c>
       <c r="F4" t="s">
-        <v>16</v>
-      </c>
-      <c r="I4"/>
+        <v>171</v>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" t="s">
-        <v>20</v>
-      </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
         <v>22</v>
       </c>
       <c r="D5" t="s">
-        <v>23</v>
+        <v>172</v>
       </c>
       <c r="E5" t="s">
-        <v>24</v>
+        <v>173</v>
       </c>
       <c r="G5" t="s">
-        <v>171</v>
-      </c>
-      <c r="I5"/>
+        <v>174</v>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" t="s">
-        <v>26</v>
-      </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
         <v>22</v>
       </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>169</v>
       </c>
       <c r="E6" t="s">
-        <v>27</v>
+        <v>170</v>
       </c>
       <c r="H6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I6"/>
+        <v>175</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" t="s">
-        <v>23</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="D7"/>
       <c r="E7" t="s">
-        <v>30</v>
-      </c>
-      <c r="G7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I7"/>
+        <v>14</v>
+      </c>
+      <c r="F7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C8" t="s">
         <v>22</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8"/>
+      <c r="E8" t="s">
         <v>23</v>
       </c>
-      <c r="E8" t="s">
-        <v>32</v>
-      </c>
-      <c r="H8" t="s">
-        <v>28</v>
-      </c>
-      <c r="I8"/>
+      <c r="G8" t="s">
+        <v>24</v>
+      </c>
+      <c r="I8" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="C9" t="s">
         <v>22</v>
       </c>
-      <c r="D9" t="s">
-        <v>23</v>
-      </c>
+      <c r="D9"/>
       <c r="E9" t="s">
-        <v>34</v>
-      </c>
-      <c r="G9" t="s">
-        <v>35</v>
-      </c>
-      <c r="I9"/>
+        <v>26</v>
+      </c>
+      <c r="H9" t="s">
+        <v>27</v>
+      </c>
+      <c r="I9" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B10" t="s">
         <v>22</v>
@@ -850,41 +850,41 @@
       <c r="C10" t="s">
         <v>22</v>
       </c>
-      <c r="D10" t="s">
-        <v>23</v>
-      </c>
+      <c r="D10"/>
       <c r="E10" t="s">
-        <v>37</v>
-      </c>
-      <c r="H10" t="s">
-        <v>38</v>
-      </c>
-      <c r="I10"/>
+        <v>29</v>
+      </c>
+      <c r="G10" t="s">
+        <v>24</v>
+      </c>
+      <c r="I10" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="B11" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>40</v>
-      </c>
-      <c r="D11" t="s">
-        <v>23</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="D11"/>
       <c r="E11" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="H11" t="s">
-        <v>42</v>
-      </c>
-      <c r="I11"/>
+        <v>27</v>
+      </c>
+      <c r="I11" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="B12" t="s">
         <v>22</v>
@@ -892,20 +892,20 @@
       <c r="C12" t="s">
         <v>22</v>
       </c>
-      <c r="D12" t="s">
-        <v>23</v>
-      </c>
+      <c r="D12"/>
       <c r="E12" t="s">
-        <v>44</v>
-      </c>
-      <c r="H12" t="s">
-        <v>45</v>
-      </c>
-      <c r="I12"/>
+        <v>33</v>
+      </c>
+      <c r="G12" t="s">
+        <v>34</v>
+      </c>
+      <c r="I12" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="B13" t="s">
         <v>22</v>
@@ -913,41 +913,41 @@
       <c r="C13" t="s">
         <v>22</v>
       </c>
-      <c r="D13" t="s">
-        <v>23</v>
-      </c>
+      <c r="D13"/>
       <c r="E13" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="H13" t="s">
-        <v>48</v>
-      </c>
-      <c r="I13"/>
+        <v>37</v>
+      </c>
+      <c r="I13" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="B14" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>22</v>
-      </c>
-      <c r="D14" t="s">
-        <v>23</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="D14"/>
       <c r="E14" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="H14" t="s">
-        <v>51</v>
-      </c>
-      <c r="I14"/>
+        <v>40</v>
+      </c>
+      <c r="I14" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="B15" t="s">
         <v>22</v>
@@ -955,20 +955,20 @@
       <c r="C15" t="s">
         <v>22</v>
       </c>
-      <c r="D15" t="s">
-        <v>23</v>
-      </c>
+      <c r="D15"/>
       <c r="E15" t="s">
-        <v>171</v>
-      </c>
-      <c r="F15" t="s">
-        <v>171</v>
-      </c>
-      <c r="I15"/>
+        <v>42</v>
+      </c>
+      <c r="H15" t="s">
+        <v>43</v>
+      </c>
+      <c r="I15" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="B16" t="s">
         <v>22</v>
@@ -976,20 +976,20 @@
       <c r="C16" t="s">
         <v>22</v>
       </c>
-      <c r="D16" t="s">
-        <v>23</v>
-      </c>
+      <c r="D16"/>
       <c r="E16" t="s">
-        <v>56</v>
-      </c>
-      <c r="G16" t="s">
-        <v>57</v>
-      </c>
-      <c r="I16"/>
+        <v>45</v>
+      </c>
+      <c r="H16" t="s">
+        <v>46</v>
+      </c>
+      <c r="I16" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="B17" t="s">
         <v>22</v>
@@ -997,20 +997,20 @@
       <c r="C17" t="s">
         <v>22</v>
       </c>
-      <c r="D17" t="s">
-        <v>23</v>
-      </c>
+      <c r="D17"/>
       <c r="E17" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="H17" t="s">
-        <v>60</v>
-      </c>
-      <c r="I17"/>
+        <v>49</v>
+      </c>
+      <c r="I17" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="B18" t="s">
         <v>22</v>
@@ -1018,20 +1018,20 @@
       <c r="C18" t="s">
         <v>22</v>
       </c>
-      <c r="D18" t="s">
-        <v>23</v>
-      </c>
+      <c r="D18"/>
       <c r="E18" t="s">
-        <v>62</v>
-      </c>
-      <c r="G18" t="s">
-        <v>63</v>
-      </c>
-      <c r="I18"/>
+        <v>51</v>
+      </c>
+      <c r="F18" t="s">
+        <v>52</v>
+      </c>
+      <c r="I18" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="B19" t="s">
         <v>22</v>
@@ -1039,20 +1039,20 @@
       <c r="C19" t="s">
         <v>22</v>
       </c>
-      <c r="D19" t="s">
-        <v>23</v>
-      </c>
+      <c r="D19"/>
       <c r="E19" t="s">
-        <v>65</v>
-      </c>
-      <c r="H19" t="s">
-        <v>66</v>
-      </c>
-      <c r="I19"/>
+        <v>54</v>
+      </c>
+      <c r="G19" t="s">
+        <v>55</v>
+      </c>
+      <c r="I19" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="B20" t="s">
         <v>22</v>
@@ -1060,20 +1060,20 @@
       <c r="C20" t="s">
         <v>22</v>
       </c>
-      <c r="D20" t="s">
-        <v>23</v>
-      </c>
+      <c r="D20"/>
       <c r="E20" t="s">
-        <v>68</v>
-      </c>
-      <c r="G20" t="s">
-        <v>35</v>
-      </c>
-      <c r="I20"/>
+        <v>57</v>
+      </c>
+      <c r="H20" t="s">
+        <v>58</v>
+      </c>
+      <c r="I20" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="B21" t="s">
         <v>22</v>
@@ -1081,20 +1081,20 @@
       <c r="C21" t="s">
         <v>22</v>
       </c>
-      <c r="D21" t="s">
-        <v>23</v>
-      </c>
+      <c r="D21"/>
       <c r="E21" t="s">
-        <v>70</v>
-      </c>
-      <c r="H21" t="s">
-        <v>71</v>
-      </c>
-      <c r="I21"/>
+        <v>60</v>
+      </c>
+      <c r="G21" t="s">
+        <v>61</v>
+      </c>
+      <c r="I21" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="B22" t="s">
         <v>22</v>
@@ -1102,20 +1102,20 @@
       <c r="C22" t="s">
         <v>22</v>
       </c>
-      <c r="D22" t="s">
-        <v>23</v>
-      </c>
+      <c r="D22"/>
       <c r="E22" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="H22" t="s">
-        <v>74</v>
-      </c>
-      <c r="I22"/>
+        <v>64</v>
+      </c>
+      <c r="I22" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="B23" t="s">
         <v>22</v>
@@ -1123,20 +1123,20 @@
       <c r="C23" t="s">
         <v>22</v>
       </c>
-      <c r="D23" t="s">
-        <v>23</v>
-      </c>
+      <c r="D23"/>
       <c r="E23" t="s">
-        <v>76</v>
-      </c>
-      <c r="H23" t="s">
-        <v>77</v>
-      </c>
-      <c r="I23"/>
+        <v>66</v>
+      </c>
+      <c r="G23" t="s">
+        <v>34</v>
+      </c>
+      <c r="I23" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="B24" t="s">
         <v>22</v>
@@ -1144,20 +1144,20 @@
       <c r="C24" t="s">
         <v>22</v>
       </c>
-      <c r="D24" t="s">
-        <v>23</v>
-      </c>
+      <c r="D24"/>
       <c r="E24" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="H24" t="s">
-        <v>80</v>
-      </c>
-      <c r="I24"/>
+        <v>69</v>
+      </c>
+      <c r="I24" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="B25" t="s">
         <v>22</v>
@@ -1165,20 +1165,20 @@
       <c r="C25" t="s">
         <v>22</v>
       </c>
-      <c r="D25" t="s">
-        <v>23</v>
-      </c>
+      <c r="D25"/>
       <c r="E25" t="s">
-        <v>82</v>
-      </c>
-      <c r="F25" t="s">
-        <v>83</v>
-      </c>
-      <c r="I25"/>
+        <v>71</v>
+      </c>
+      <c r="H25" t="s">
+        <v>72</v>
+      </c>
+      <c r="I25" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="B26" t="s">
         <v>22</v>
@@ -1186,20 +1186,20 @@
       <c r="C26" t="s">
         <v>22</v>
       </c>
-      <c r="D26" t="s">
-        <v>23</v>
-      </c>
+      <c r="D26"/>
       <c r="E26" t="s">
-        <v>85</v>
-      </c>
-      <c r="G26" t="s">
-        <v>57</v>
-      </c>
-      <c r="I26"/>
+        <v>74</v>
+      </c>
+      <c r="H26" t="s">
+        <v>75</v>
+      </c>
+      <c r="I26" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="B27" t="s">
         <v>22</v>
@@ -1207,20 +1207,20 @@
       <c r="C27" t="s">
         <v>22</v>
       </c>
-      <c r="D27" t="s">
-        <v>23</v>
-      </c>
+      <c r="D27"/>
       <c r="E27" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="H27" t="s">
-        <v>88</v>
-      </c>
-      <c r="I27"/>
+        <v>78</v>
+      </c>
+      <c r="I27" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="B28" t="s">
         <v>22</v>
@@ -1228,20 +1228,20 @@
       <c r="C28" t="s">
         <v>22</v>
       </c>
-      <c r="D28" t="s">
-        <v>23</v>
-      </c>
+      <c r="D28"/>
       <c r="E28" t="s">
-        <v>90</v>
-      </c>
-      <c r="G28" t="s">
-        <v>63</v>
-      </c>
-      <c r="I28"/>
+        <v>80</v>
+      </c>
+      <c r="F28" t="s">
+        <v>81</v>
+      </c>
+      <c r="I28" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="B29" t="s">
         <v>22</v>
@@ -1249,20 +1249,20 @@
       <c r="C29" t="s">
         <v>22</v>
       </c>
-      <c r="D29" t="s">
-        <v>23</v>
-      </c>
+      <c r="D29"/>
       <c r="E29" t="s">
-        <v>92</v>
-      </c>
-      <c r="H29" t="s">
-        <v>93</v>
-      </c>
-      <c r="I29"/>
+        <v>83</v>
+      </c>
+      <c r="G29" t="s">
+        <v>55</v>
+      </c>
+      <c r="I29" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="B30" t="s">
         <v>22</v>
@@ -1270,20 +1270,20 @@
       <c r="C30" t="s">
         <v>22</v>
       </c>
-      <c r="D30" t="s">
-        <v>23</v>
-      </c>
+      <c r="D30"/>
       <c r="E30" t="s">
-        <v>95</v>
-      </c>
-      <c r="G30" t="s">
-        <v>35</v>
-      </c>
-      <c r="I30"/>
+        <v>85</v>
+      </c>
+      <c r="H30" t="s">
+        <v>86</v>
+      </c>
+      <c r="I30" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="B31" t="s">
         <v>22</v>
@@ -1291,20 +1291,20 @@
       <c r="C31" t="s">
         <v>22</v>
       </c>
-      <c r="D31" t="s">
-        <v>23</v>
-      </c>
+      <c r="D31"/>
       <c r="E31" t="s">
-        <v>97</v>
-      </c>
-      <c r="H31" t="s">
-        <v>98</v>
-      </c>
-      <c r="I31"/>
+        <v>88</v>
+      </c>
+      <c r="G31" t="s">
+        <v>61</v>
+      </c>
+      <c r="I31" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="B32" t="s">
         <v>22</v>
@@ -1312,20 +1312,20 @@
       <c r="C32" t="s">
         <v>22</v>
       </c>
-      <c r="D32" t="s">
-        <v>23</v>
-      </c>
+      <c r="D32"/>
       <c r="E32" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="H32" t="s">
-        <v>101</v>
-      </c>
-      <c r="I32"/>
+        <v>91</v>
+      </c>
+      <c r="I32" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="B33" t="s">
         <v>22</v>
@@ -1333,20 +1333,20 @@
       <c r="C33" t="s">
         <v>22</v>
       </c>
-      <c r="D33" t="s">
-        <v>23</v>
-      </c>
+      <c r="D33"/>
       <c r="E33" t="s">
-        <v>103</v>
-      </c>
-      <c r="F33" t="s">
-        <v>104</v>
-      </c>
-      <c r="I33"/>
+        <v>93</v>
+      </c>
+      <c r="G33" t="s">
+        <v>34</v>
+      </c>
+      <c r="I33" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="B34" t="s">
         <v>22</v>
@@ -1354,20 +1354,20 @@
       <c r="C34" t="s">
         <v>22</v>
       </c>
-      <c r="D34" t="s">
-        <v>23</v>
-      </c>
+      <c r="D34"/>
       <c r="E34" t="s">
-        <v>106</v>
-      </c>
-      <c r="F34" t="s">
-        <v>57</v>
-      </c>
-      <c r="I34"/>
+        <v>95</v>
+      </c>
+      <c r="H34" t="s">
+        <v>96</v>
+      </c>
+      <c r="I34" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="B35" t="s">
         <v>22</v>
@@ -1375,20 +1375,20 @@
       <c r="C35" t="s">
         <v>22</v>
       </c>
-      <c r="D35" t="s">
-        <v>23</v>
-      </c>
+      <c r="D35"/>
       <c r="E35" t="s">
-        <v>108</v>
-      </c>
-      <c r="G35" t="s">
-        <v>109</v>
-      </c>
-      <c r="I35"/>
+        <v>98</v>
+      </c>
+      <c r="H35" t="s">
+        <v>99</v>
+      </c>
+      <c r="I35" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="B36" t="s">
         <v>22</v>
@@ -1396,20 +1396,20 @@
       <c r="C36" t="s">
         <v>22</v>
       </c>
-      <c r="D36" t="s">
-        <v>23</v>
-      </c>
+      <c r="D36"/>
       <c r="E36" t="s">
-        <v>111</v>
-      </c>
-      <c r="H36" t="s">
-        <v>112</v>
-      </c>
-      <c r="I36"/>
+        <v>101</v>
+      </c>
+      <c r="F36" t="s">
+        <v>102</v>
+      </c>
+      <c r="I36" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="B37" t="s">
         <v>22</v>
@@ -1417,20 +1417,20 @@
       <c r="C37" t="s">
         <v>22</v>
       </c>
-      <c r="D37" t="s">
-        <v>23</v>
-      </c>
+      <c r="D37"/>
       <c r="E37" t="s">
-        <v>114</v>
-      </c>
-      <c r="G37" t="s">
-        <v>54</v>
-      </c>
-      <c r="I37"/>
+        <v>104</v>
+      </c>
+      <c r="F37" t="s">
+        <v>55</v>
+      </c>
+      <c r="I37" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="B38" t="s">
         <v>22</v>
@@ -1438,20 +1438,20 @@
       <c r="C38" t="s">
         <v>22</v>
       </c>
-      <c r="D38" t="s">
-        <v>23</v>
-      </c>
+      <c r="D38"/>
       <c r="E38" t="s">
-        <v>116</v>
-      </c>
-      <c r="H38" t="s">
-        <v>60</v>
-      </c>
-      <c r="I38"/>
+        <v>106</v>
+      </c>
+      <c r="G38" t="s">
+        <v>107</v>
+      </c>
+      <c r="I38" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="B39" t="s">
         <v>22</v>
@@ -1459,20 +1459,20 @@
       <c r="C39" t="s">
         <v>22</v>
       </c>
-      <c r="D39" t="s">
-        <v>23</v>
-      </c>
+      <c r="D39"/>
       <c r="E39" t="s">
-        <v>118</v>
-      </c>
-      <c r="G39" t="s">
-        <v>83</v>
-      </c>
-      <c r="I39"/>
+        <v>109</v>
+      </c>
+      <c r="H39" t="s">
+        <v>110</v>
+      </c>
+      <c r="I39" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="B40" t="s">
         <v>22</v>
@@ -1480,20 +1480,20 @@
       <c r="C40" t="s">
         <v>22</v>
       </c>
-      <c r="D40" t="s">
-        <v>23</v>
-      </c>
+      <c r="D40"/>
       <c r="E40" t="s">
-        <v>120</v>
-      </c>
-      <c r="H40" t="s">
-        <v>88</v>
-      </c>
-      <c r="I40"/>
+        <v>112</v>
+      </c>
+      <c r="G40" t="s">
+        <v>52</v>
+      </c>
+      <c r="I40" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="B41" t="s">
         <v>22</v>
@@ -1501,20 +1501,20 @@
       <c r="C41" t="s">
         <v>22</v>
       </c>
-      <c r="D41" t="s">
-        <v>23</v>
-      </c>
+      <c r="D41"/>
       <c r="E41" t="s">
-        <v>122</v>
-      </c>
-      <c r="G41" t="s">
-        <v>123</v>
-      </c>
-      <c r="I41"/>
+        <v>114</v>
+      </c>
+      <c r="H41" t="s">
+        <v>58</v>
+      </c>
+      <c r="I41" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="B42" t="s">
         <v>22</v>
@@ -1522,20 +1522,20 @@
       <c r="C42" t="s">
         <v>22</v>
       </c>
-      <c r="D42" t="s">
-        <v>23</v>
-      </c>
+      <c r="D42"/>
       <c r="E42" t="s">
-        <v>125</v>
-      </c>
-      <c r="F42" t="s">
-        <v>63</v>
-      </c>
-      <c r="I42"/>
+        <v>116</v>
+      </c>
+      <c r="G42" t="s">
+        <v>81</v>
+      </c>
+      <c r="I42" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="B43" t="s">
         <v>22</v>
@@ -1543,20 +1543,20 @@
       <c r="C43" t="s">
         <v>22</v>
       </c>
-      <c r="D43" t="s">
-        <v>23</v>
-      </c>
+      <c r="D43"/>
       <c r="E43" t="s">
-        <v>127</v>
-      </c>
-      <c r="G43" t="s">
-        <v>109</v>
-      </c>
-      <c r="I43"/>
+        <v>118</v>
+      </c>
+      <c r="H43" t="s">
+        <v>86</v>
+      </c>
+      <c r="I43" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="B44" t="s">
         <v>22</v>
@@ -1564,20 +1564,20 @@
       <c r="C44" t="s">
         <v>22</v>
       </c>
-      <c r="D44" t="s">
-        <v>23</v>
-      </c>
+      <c r="D44"/>
       <c r="E44" t="s">
-        <v>129</v>
-      </c>
-      <c r="H44" t="s">
-        <v>130</v>
-      </c>
-      <c r="I44"/>
+        <v>120</v>
+      </c>
+      <c r="G44" t="s">
+        <v>121</v>
+      </c>
+      <c r="I44" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="B45" t="s">
         <v>22</v>
@@ -1585,20 +1585,20 @@
       <c r="C45" t="s">
         <v>22</v>
       </c>
-      <c r="D45" t="s">
-        <v>23</v>
-      </c>
+      <c r="D45"/>
       <c r="E45" t="s">
-        <v>132</v>
-      </c>
-      <c r="G45" t="s">
-        <v>54</v>
-      </c>
-      <c r="I45"/>
+        <v>123</v>
+      </c>
+      <c r="F45" t="s">
+        <v>61</v>
+      </c>
+      <c r="I45" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="B46" t="s">
         <v>22</v>
@@ -1606,20 +1606,20 @@
       <c r="C46" t="s">
         <v>22</v>
       </c>
-      <c r="D46" t="s">
-        <v>23</v>
-      </c>
+      <c r="D46"/>
       <c r="E46" t="s">
-        <v>134</v>
-      </c>
-      <c r="H46" t="s">
-        <v>66</v>
-      </c>
-      <c r="I46"/>
+        <v>125</v>
+      </c>
+      <c r="G46" t="s">
+        <v>107</v>
+      </c>
+      <c r="I46" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="B47" t="s">
         <v>22</v>
@@ -1627,20 +1627,20 @@
       <c r="C47" t="s">
         <v>22</v>
       </c>
-      <c r="D47" t="s">
-        <v>23</v>
-      </c>
+      <c r="D47"/>
       <c r="E47" t="s">
-        <v>136</v>
-      </c>
-      <c r="G47" t="s">
-        <v>83</v>
-      </c>
-      <c r="I47"/>
+        <v>127</v>
+      </c>
+      <c r="H47" t="s">
+        <v>128</v>
+      </c>
+      <c r="I47" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="B48" t="s">
         <v>22</v>
@@ -1648,20 +1648,20 @@
       <c r="C48" t="s">
         <v>22</v>
       </c>
-      <c r="D48" t="s">
-        <v>23</v>
-      </c>
+      <c r="D48"/>
       <c r="E48" t="s">
-        <v>138</v>
-      </c>
-      <c r="H48" t="s">
-        <v>93</v>
-      </c>
-      <c r="I48"/>
+        <v>130</v>
+      </c>
+      <c r="G48" t="s">
+        <v>52</v>
+      </c>
+      <c r="I48" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="B49" t="s">
         <v>22</v>
@@ -1669,20 +1669,20 @@
       <c r="C49" t="s">
         <v>22</v>
       </c>
-      <c r="D49" t="s">
-        <v>23</v>
-      </c>
+      <c r="D49"/>
       <c r="E49" t="s">
-        <v>140</v>
-      </c>
-      <c r="G49" t="s">
-        <v>123</v>
-      </c>
-      <c r="I49"/>
+        <v>132</v>
+      </c>
+      <c r="H49" t="s">
+        <v>64</v>
+      </c>
+      <c r="I49" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="B50" t="s">
         <v>22</v>
@@ -1690,20 +1690,20 @@
       <c r="C50" t="s">
         <v>22</v>
       </c>
-      <c r="D50" t="s">
-        <v>23</v>
-      </c>
+      <c r="D50"/>
       <c r="E50" t="s">
-        <v>142</v>
-      </c>
-      <c r="F50" t="s">
-        <v>35</v>
-      </c>
-      <c r="I50"/>
+        <v>134</v>
+      </c>
+      <c r="G50" t="s">
+        <v>81</v>
+      </c>
+      <c r="I50" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="B51" t="s">
         <v>22</v>
@@ -1711,20 +1711,20 @@
       <c r="C51" t="s">
         <v>22</v>
       </c>
-      <c r="D51" t="s">
-        <v>23</v>
-      </c>
+      <c r="D51"/>
       <c r="E51" t="s">
-        <v>144</v>
-      </c>
-      <c r="G51" t="s">
-        <v>109</v>
-      </c>
-      <c r="I51"/>
+        <v>136</v>
+      </c>
+      <c r="H51" t="s">
+        <v>91</v>
+      </c>
+      <c r="I51" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="B52" t="s">
         <v>22</v>
@@ -1732,20 +1732,20 @@
       <c r="C52" t="s">
         <v>22</v>
       </c>
-      <c r="D52" t="s">
-        <v>23</v>
-      </c>
+      <c r="D52"/>
       <c r="E52" t="s">
-        <v>146</v>
-      </c>
-      <c r="H52" t="s">
-        <v>38</v>
-      </c>
-      <c r="I52"/>
+        <v>138</v>
+      </c>
+      <c r="G52" t="s">
+        <v>121</v>
+      </c>
+      <c r="I52" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="B53" t="s">
         <v>22</v>
@@ -1753,20 +1753,20 @@
       <c r="C53" t="s">
         <v>22</v>
       </c>
-      <c r="D53" t="s">
-        <v>23</v>
-      </c>
+      <c r="D53"/>
       <c r="E53" t="s">
-        <v>148</v>
-      </c>
-      <c r="H53" t="s">
-        <v>42</v>
-      </c>
-      <c r="I53"/>
+        <v>140</v>
+      </c>
+      <c r="F53" t="s">
+        <v>34</v>
+      </c>
+      <c r="I53" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="B54" t="s">
         <v>22</v>
@@ -1774,20 +1774,20 @@
       <c r="C54" t="s">
         <v>22</v>
       </c>
-      <c r="D54" t="s">
-        <v>23</v>
-      </c>
+      <c r="D54"/>
       <c r="E54" t="s">
-        <v>150</v>
-      </c>
-      <c r="H54" t="s">
-        <v>45</v>
-      </c>
-      <c r="I54"/>
+        <v>142</v>
+      </c>
+      <c r="G54" t="s">
+        <v>107</v>
+      </c>
+      <c r="I54" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="B55" t="s">
         <v>22</v>
@@ -1795,20 +1795,20 @@
       <c r="C55" t="s">
         <v>22</v>
       </c>
-      <c r="D55" t="s">
-        <v>23</v>
-      </c>
+      <c r="D55"/>
       <c r="E55" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="H55" t="s">
-        <v>48</v>
-      </c>
-      <c r="I55"/>
+        <v>37</v>
+      </c>
+      <c r="I55" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="B56" t="s">
         <v>22</v>
@@ -1816,20 +1816,20 @@
       <c r="C56" t="s">
         <v>22</v>
       </c>
-      <c r="D56" t="s">
-        <v>23</v>
-      </c>
+      <c r="D56"/>
       <c r="E56" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="H56" t="s">
-        <v>51</v>
-      </c>
-      <c r="I56"/>
+        <v>40</v>
+      </c>
+      <c r="I56" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="B57" t="s">
         <v>22</v>
@@ -1837,20 +1837,20 @@
       <c r="C57" t="s">
         <v>22</v>
       </c>
-      <c r="D57" t="s">
-        <v>23</v>
-      </c>
+      <c r="D57"/>
       <c r="E57" t="s">
-        <v>156</v>
-      </c>
-      <c r="G57" t="s">
-        <v>54</v>
-      </c>
-      <c r="I57"/>
+        <v>148</v>
+      </c>
+      <c r="H57" t="s">
+        <v>43</v>
+      </c>
+      <c r="I57" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="B58" t="s">
         <v>22</v>
@@ -1858,20 +1858,20 @@
       <c r="C58" t="s">
         <v>22</v>
       </c>
-      <c r="D58" t="s">
-        <v>23</v>
-      </c>
+      <c r="D58"/>
       <c r="E58" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="H58" t="s">
-        <v>71</v>
-      </c>
-      <c r="I58"/>
+        <v>46</v>
+      </c>
+      <c r="I58" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B59" t="s">
         <v>22</v>
@@ -1879,20 +1879,20 @@
       <c r="C59" t="s">
         <v>22</v>
       </c>
-      <c r="D59" t="s">
-        <v>23</v>
-      </c>
+      <c r="D59"/>
       <c r="E59" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="H59" t="s">
-        <v>74</v>
-      </c>
-      <c r="I59"/>
+        <v>49</v>
+      </c>
+      <c r="I59" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="B60" t="s">
         <v>22</v>
@@ -1900,20 +1900,20 @@
       <c r="C60" t="s">
         <v>22</v>
       </c>
-      <c r="D60" t="s">
-        <v>23</v>
-      </c>
+      <c r="D60"/>
       <c r="E60" t="s">
-        <v>162</v>
-      </c>
-      <c r="H60" t="s">
-        <v>77</v>
-      </c>
-      <c r="I60"/>
+        <v>154</v>
+      </c>
+      <c r="G60" t="s">
+        <v>52</v>
+      </c>
+      <c r="I60" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="B61" t="s">
         <v>22</v>
@@ -1921,20 +1921,20 @@
       <c r="C61" t="s">
         <v>22</v>
       </c>
-      <c r="D61" t="s">
-        <v>23</v>
-      </c>
+      <c r="D61"/>
       <c r="E61" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="H61" t="s">
-        <v>80</v>
-      </c>
-      <c r="I61"/>
+        <v>69</v>
+      </c>
+      <c r="I61" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="B62" t="s">
         <v>22</v>
@@ -1942,20 +1942,20 @@
       <c r="C62" t="s">
         <v>22</v>
       </c>
-      <c r="D62" t="s">
-        <v>23</v>
-      </c>
+      <c r="D62"/>
       <c r="E62" t="s">
-        <v>166</v>
-      </c>
-      <c r="G62" t="s">
-        <v>83</v>
-      </c>
-      <c r="I62"/>
+        <v>158</v>
+      </c>
+      <c r="H62" t="s">
+        <v>72</v>
+      </c>
+      <c r="I62" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="B63" t="s">
         <v>22</v>
@@ -1963,20 +1963,20 @@
       <c r="C63" t="s">
         <v>22</v>
       </c>
-      <c r="D63" t="s">
-        <v>23</v>
-      </c>
+      <c r="D63"/>
       <c r="E63" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="H63" t="s">
-        <v>98</v>
-      </c>
-      <c r="I63"/>
+        <v>75</v>
+      </c>
+      <c r="I63" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="B64" t="s">
         <v>22</v>
@@ -1984,16 +1984,79 @@
       <c r="C64" t="s">
         <v>22</v>
       </c>
-      <c r="D64" t="s">
-        <v>23</v>
-      </c>
+      <c r="D64"/>
       <c r="E64" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="H64" t="s">
-        <v>101</v>
-      </c>
-      <c r="I64"/>
+        <v>78</v>
+      </c>
+      <c r="I64" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s">
+        <v>163</v>
+      </c>
+      <c r="B65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C65" t="s">
+        <v>22</v>
+      </c>
+      <c r="D65"/>
+      <c r="E65" t="s">
+        <v>164</v>
+      </c>
+      <c r="G65" t="s">
+        <v>81</v>
+      </c>
+      <c r="I65" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="s">
+        <v>165</v>
+      </c>
+      <c r="B66" t="s">
+        <v>22</v>
+      </c>
+      <c r="C66" t="s">
+        <v>22</v>
+      </c>
+      <c r="D66"/>
+      <c r="E66" t="s">
+        <v>166</v>
+      </c>
+      <c r="H66" t="s">
+        <v>96</v>
+      </c>
+      <c r="I66" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="s">
+        <v>167</v>
+      </c>
+      <c r="B67" t="s">
+        <v>22</v>
+      </c>
+      <c r="C67" t="s">
+        <v>22</v>
+      </c>
+      <c r="D67"/>
+      <c r="E67" t="s">
+        <v>168</v>
+      </c>
+      <c r="H67" t="s">
+        <v>99</v>
+      </c>
+      <c r="I67" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>